<commit_message>
fixed test for robot_assembly
</commit_message>
<xml_diff>
--- a/tests/files_for_testing/Random_PCR_list.xlsx
+++ b/tests/files_for_testing/Random_PCR_list.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucaslevassor/projects/teemi/tests/files_for_testing/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F593FE89-9FEE-3942-A4BB-B2B5ADDDBA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -19,9 +25,6 @@
     <t>PCR#</t>
   </si>
   <si>
-    <t>Template</t>
-  </si>
-  <si>
     <t>forward_primer</t>
   </si>
   <si>
@@ -167,13 +170,16 @@
   </si>
   <si>
     <t>R00177</t>
+  </si>
+  <si>
+    <t>template</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,13 +242,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -280,7 +294,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -314,6 +328,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -348,9 +363,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -523,48 +539,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>167</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2">
         <v>55.21</v>
@@ -573,21 +591,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3">
         <v>55.21</v>
@@ -596,21 +614,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4">
         <v>55.21</v>
@@ -619,21 +637,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5">
         <v>55.21</v>
@@ -642,21 +660,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>223</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6">
         <v>55.21</v>
@@ -665,21 +683,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>224</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7">
         <v>55.21</v>
@@ -688,21 +706,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>225</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8">
         <v>55.21</v>
@@ -711,21 +729,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>226</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9">
         <v>55.21</v>
@@ -734,21 +752,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>243</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10">
         <v>55.21</v>
@@ -757,21 +775,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>244</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11">
         <v>55.21</v>
@@ -780,21 +798,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>245</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F12">
         <v>55.21</v>
@@ -803,21 +821,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>246</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13">
         <v>55.21</v>
@@ -826,21 +844,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>263</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14">
         <v>55.21</v>
@@ -849,21 +867,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>264</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15">
         <v>55.21</v>
@@ -872,21 +890,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>265</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F16">
         <v>55.21</v>
@@ -895,21 +913,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>266</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17">
         <v>55.21</v>
@@ -918,21 +936,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>283</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18">
         <v>55.21</v>
@@ -941,21 +959,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>284</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19">
         <v>55.21</v>
@@ -964,21 +982,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>285</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F20">
         <v>55.21</v>
@@ -987,21 +1005,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>286</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F21">
         <v>55.21</v>
@@ -1010,21 +1028,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>303</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F22">
         <v>55.21</v>
@@ -1033,21 +1051,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>304</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23">
         <v>55.21</v>
@@ -1056,21 +1074,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>305</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F24">
         <v>55.21</v>
@@ -1079,21 +1097,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>306</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F25">
         <v>55.21</v>
@@ -1102,21 +1120,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>323</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F26">
         <v>55.21</v>
@@ -1125,21 +1143,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>324</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F27">
         <v>55.21</v>
@@ -1148,21 +1166,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>325</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F28">
         <v>55.21</v>
@@ -1171,21 +1189,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>326</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F29">
         <v>55.21</v>
@@ -1194,22 +1212,22 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>343</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" t="s">
         <v>46</v>
       </c>
-      <c r="E30" t="s">
-        <v>47</v>
-      </c>
       <c r="F30">
         <v>55.21</v>
       </c>
@@ -1217,21 +1235,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>344</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F31">
         <v>55.21</v>
@@ -1240,21 +1258,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>345</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F32">
         <v>55.21</v>
@@ -1263,21 +1281,21 @@
         <v>55.21</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>346</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F33">
         <v>55.21</v>

</xml_diff>